<commit_message>
asset profile changes commit
</commit_message>
<xml_diff>
--- a/TestData/Input.xlsx
+++ b/TestData/Input.xlsx
@@ -84,9 +84,6 @@
     <t>Department</t>
   </si>
   <si>
-    <t>Auto-1</t>
-  </si>
-  <si>
     <t>New</t>
   </si>
   <si>
@@ -96,12 +93,6 @@
     <t>default</t>
   </si>
   <si>
-    <t>Division1-Division1</t>
-  </si>
-  <si>
-    <t>SDiv01-SDiv01</t>
-  </si>
-  <si>
     <t>Lc-00252</t>
   </si>
   <si>
@@ -114,7 +105,16 @@
     <t>Car</t>
   </si>
   <si>
-    <t>0017-0017</t>
+    <t>ddd - ddd</t>
+  </si>
+  <si>
+    <t>sss - sss</t>
+  </si>
+  <si>
+    <t>aaa</t>
+  </si>
+  <si>
+    <t>Auto-13</t>
   </si>
 </sst>
 </file>
@@ -179,13 +179,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -552,7 +555,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -605,37 +608,37 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="D2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="G2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Lease Profile final commit and ltr to ar job initial commit
</commit_message>
<xml_diff>
--- a/TestData/Input.xlsx
+++ b/TestData/Input.xlsx
@@ -15,7 +15,7 @@
     <sheet name="credentials" sheetId="1" r:id="rId1"/>
     <sheet name="AssetProfile" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -114,7 +114,7 @@
     <t>aaa</t>
   </si>
   <si>
-    <t>Auto-32</t>
+    <t>Auto-57</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
changes into switch window control commit
</commit_message>
<xml_diff>
--- a/TestData/Input.xlsx
+++ b/TestData/Input.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="76">
   <si>
     <t>Company Name</t>
   </si>
@@ -136,139 +136,124 @@
     <t>Cost</t>
   </si>
   <si>
-    <t>Auto-306</t>
-  </si>
-  <si>
-    <t>Auto-307</t>
-  </si>
-  <si>
-    <t>Auto-308</t>
-  </si>
-  <si>
-    <t>Auto-309</t>
-  </si>
-  <si>
-    <t>Auto-310</t>
-  </si>
-  <si>
-    <t>Auto-311</t>
-  </si>
-  <si>
-    <t>Auto-312</t>
-  </si>
-  <si>
-    <t>Auto-313</t>
-  </si>
-  <si>
-    <t>Auto-314</t>
-  </si>
-  <si>
-    <t>Auto-315</t>
-  </si>
-  <si>
-    <t>Auto-316</t>
-  </si>
-  <si>
-    <t>Auto-317</t>
-  </si>
-  <si>
-    <t>Auto-318</t>
-  </si>
-  <si>
-    <t>Auto-319</t>
-  </si>
-  <si>
-    <t>Auto-320</t>
-  </si>
-  <si>
-    <t>Auto-321</t>
-  </si>
-  <si>
-    <t>Auto-322</t>
-  </si>
-  <si>
-    <t>Auto-323</t>
-  </si>
-  <si>
-    <t>Auto-324</t>
-  </si>
-  <si>
-    <t>Auto-325</t>
-  </si>
-  <si>
-    <t>Auto-326</t>
-  </si>
-  <si>
-    <t>Auto-327</t>
-  </si>
-  <si>
-    <t>Auto-328</t>
-  </si>
-  <si>
-    <t>Auto-329</t>
-  </si>
-  <si>
-    <t>Auto-330</t>
-  </si>
-  <si>
-    <t>Auto-331</t>
-  </si>
-  <si>
-    <t>Auto-332</t>
-  </si>
-  <si>
-    <t>Auto-333</t>
-  </si>
-  <si>
-    <t>Auto-334</t>
-  </si>
-  <si>
-    <t>Auto-335</t>
-  </si>
-  <si>
-    <t>Auto-336</t>
-  </si>
-  <si>
-    <t>Auto-337</t>
-  </si>
-  <si>
-    <t>Auto-338</t>
-  </si>
-  <si>
-    <t>Auto-339</t>
-  </si>
-  <si>
-    <t>Auto-340</t>
-  </si>
-  <si>
-    <t>Auto-341</t>
-  </si>
-  <si>
-    <t>Auto-342</t>
-  </si>
-  <si>
-    <t>Auto-343</t>
-  </si>
-  <si>
-    <t>Auto-344</t>
-  </si>
-  <si>
-    <t>Auto-345</t>
-  </si>
-  <si>
-    <t>Auto-346</t>
-  </si>
-  <si>
-    <t>Auto-347</t>
-  </si>
-  <si>
-    <t>Auto-348</t>
-  </si>
-  <si>
-    <t>Auto-349</t>
-  </si>
-  <si>
-    <t>Auto-350</t>
+    <t>Auto-441</t>
+  </si>
+  <si>
+    <t>Auto-442</t>
+  </si>
+  <si>
+    <t>Auto-443</t>
+  </si>
+  <si>
+    <t>Auto-444</t>
+  </si>
+  <si>
+    <t>Auto-445</t>
+  </si>
+  <si>
+    <t>Auto-446</t>
+  </si>
+  <si>
+    <t>Auto-447</t>
+  </si>
+  <si>
+    <t>Auto-448</t>
+  </si>
+  <si>
+    <t>Auto-449</t>
+  </si>
+  <si>
+    <t>Auto-450</t>
+  </si>
+  <si>
+    <t>Auto-451</t>
+  </si>
+  <si>
+    <t>Auto-452</t>
+  </si>
+  <si>
+    <t>Auto-453</t>
+  </si>
+  <si>
+    <t>Auto-454</t>
+  </si>
+  <si>
+    <t>Auto-455</t>
+  </si>
+  <si>
+    <t>Auto-456</t>
+  </si>
+  <si>
+    <t>Auto-457</t>
+  </si>
+  <si>
+    <t>Auto-458</t>
+  </si>
+  <si>
+    <t>Auto-459</t>
+  </si>
+  <si>
+    <t>Auto-501</t>
+  </si>
+  <si>
+    <t>Auto-502</t>
+  </si>
+  <si>
+    <t>Auto-503</t>
+  </si>
+  <si>
+    <t>Auto-504</t>
+  </si>
+  <si>
+    <t>Auto-505</t>
+  </si>
+  <si>
+    <t>Auto-506</t>
+  </si>
+  <si>
+    <t>Auto-507</t>
+  </si>
+  <si>
+    <t>Auto-508</t>
+  </si>
+  <si>
+    <t>Auto-509</t>
+  </si>
+  <si>
+    <t>Auto-510</t>
+  </si>
+  <si>
+    <t>Auto-511</t>
+  </si>
+  <si>
+    <t>Auto-512</t>
+  </si>
+  <si>
+    <t>Auto-513</t>
+  </si>
+  <si>
+    <t>Auto-514</t>
+  </si>
+  <si>
+    <t>Auto-515</t>
+  </si>
+  <si>
+    <t>Auto-516</t>
+  </si>
+  <si>
+    <t>Auto-517</t>
+  </si>
+  <si>
+    <t>Auto-518</t>
+  </si>
+  <si>
+    <t>Auto-519</t>
+  </si>
+  <si>
+    <t>Auto-520</t>
+  </si>
+  <si>
+    <t>Auto-521</t>
   </si>
 </sst>
 </file>
@@ -355,7 +340,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -368,7 +353,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -736,10 +720,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L52"/>
+  <dimension ref="A1:L60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A6"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -795,7 +779,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>24</v>
@@ -833,7 +817,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>24</v>
@@ -871,7 +855,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="L4" s="3">
         <v>300</v>
@@ -879,7 +863,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="L5" s="3">
         <v>400</v>
@@ -887,7 +871,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="L6" s="3">
         <v>500</v>
@@ -895,7 +879,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="L7" s="3">
         <v>600</v>
@@ -903,7 +887,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="L8" s="3">
         <v>700</v>
@@ -911,7 +895,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="L9" s="3">
         <v>800</v>
@@ -919,7 +903,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="L10" s="3">
         <v>900</v>
@@ -927,7 +911,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="L11" s="3">
         <v>1000</v>
@@ -935,7 +919,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="L12" s="3">
         <v>1001</v>
@@ -943,7 +927,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>41</v>
+        <v>66</v>
       </c>
       <c r="L13" s="3">
         <v>1002</v>
@@ -951,7 +935,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="L14" s="3">
         <v>1003</v>
@@ -959,7 +943,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="L15" s="3">
         <v>1004</v>
@@ -967,7 +951,7 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>44</v>
+        <v>69</v>
       </c>
       <c r="L16" s="3">
         <v>1005</v>
@@ -975,7 +959,7 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="L17" s="3">
         <v>1006</v>
@@ -983,7 +967,7 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>46</v>
+        <v>71</v>
       </c>
       <c r="L18" s="3">
         <v>1007</v>
@@ -991,7 +975,7 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>47</v>
+        <v>72</v>
       </c>
       <c r="L19" s="3">
         <v>1008</v>
@@ -999,7 +983,7 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>48</v>
+        <v>73</v>
       </c>
       <c r="L20" s="3">
         <v>1009</v>
@@ -1007,7 +991,7 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>49</v>
+        <v>74</v>
       </c>
       <c r="L21" s="3">
         <v>1010</v>
@@ -1015,167 +999,110 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="L22" s="3">
         <v>1011</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="L23" s="3">
         <v>1012</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="L24" s="3">
         <v>1013</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="L25" s="3">
         <v>1014</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="L26" s="3">
         <v>1015</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="L27" s="3">
         <v>1016</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="L28" s="3">
         <v>1017</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="L29" s="3">
         <v>1018</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="L30" s="3">
         <v>1019</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="L31" s="3">
         <v>1020</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="L32" s="3">
         <v>1021</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="L33" s="3">
         <v>1022</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="L34" s="3">
         <v>1023</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="L35" s="3">
         <v>1024</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="L36" s="3">
         <v>1025</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>65</v>
-      </c>
       <c r="L37" s="3">
         <v>1026</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="L38" s="3">
         <v>1027</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>67</v>
-      </c>
       <c r="L39" s="3">
         <v>1028</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>68</v>
-      </c>
       <c r="L40" s="3">
         <v>1029</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="L41" s="3">
         <v>1030</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>70</v>
+        <v>36</v>
       </c>
       <c r="L42" s="3">
         <v>1031</v>
@@ -1183,7 +1110,7 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>71</v>
+        <v>37</v>
       </c>
       <c r="L43" s="3">
         <v>1032</v>
@@ -1191,7 +1118,7 @@
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>72</v>
+        <v>38</v>
       </c>
       <c r="L44" s="3">
         <v>1033</v>
@@ -1199,7 +1126,7 @@
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>73</v>
+        <v>39</v>
       </c>
       <c r="L45" s="3">
         <v>1034</v>
@@ -1207,7 +1134,7 @@
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>74</v>
+        <v>40</v>
       </c>
       <c r="L46" s="3">
         <v>1035</v>
@@ -1215,7 +1142,7 @@
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="L47" s="3">
         <v>1036</v>
@@ -1223,7 +1150,7 @@
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>76</v>
+        <v>42</v>
       </c>
       <c r="L48" s="3">
         <v>1037</v>
@@ -1231,7 +1158,7 @@
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>77</v>
+        <v>43</v>
       </c>
       <c r="L49" s="3">
         <v>1038</v>
@@ -1239,7 +1166,7 @@
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>78</v>
+        <v>44</v>
       </c>
       <c r="L50" s="3">
         <v>1039</v>
@@ -1247,15 +1174,79 @@
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>79</v>
+        <v>45</v>
       </c>
       <c r="L51" s="3">
         <v>1040</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A52" s="8" t="s">
-        <v>80</v>
+      <c r="A52" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L52" s="3">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="L53" s="3">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="L54" s="3">
+        <v>1043</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L55" s="3">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L56" s="3">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="L57" s="3">
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="L58" s="3">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L59" s="3">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Demo AutomationFrame work release 1
</commit_message>
<xml_diff>
--- a/TestData/Input.xlsx
+++ b/TestData/Input.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\amar\Automation\MyFirstAutomation-Backup\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\amar\OdessaAutomationDemo\LeaseWave4.0AutomationFrameWorkDemo\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -175,22 +175,22 @@
     <t>Annually</t>
   </si>
   <si>
-    <t>Demo-303</t>
-  </si>
-  <si>
-    <t>Demo-304</t>
-  </si>
-  <si>
-    <t>Demo-305</t>
-  </si>
-  <si>
-    <t>Demo-306</t>
-  </si>
-  <si>
-    <t>Demo-307</t>
-  </si>
-  <si>
-    <t>Demo-308</t>
+    <t>Demo-322</t>
+  </si>
+  <si>
+    <t>Demo-323</t>
+  </si>
+  <si>
+    <t>Demo-324</t>
+  </si>
+  <si>
+    <t>Demo-325</t>
+  </si>
+  <si>
+    <t>Demo-326</t>
+  </si>
+  <si>
+    <t>Demo-327</t>
   </si>
 </sst>
 </file>
@@ -660,7 +660,7 @@
   <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A2" sqref="A2:A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>